<commit_message>
0.7 voor review; 0.6 afgesloten
</commit_message>
<xml_diff>
--- a/3. waardelijsten/IMKL2015 - 0.6 waardelijsten.xlsx
+++ b/3. waardelijsten/IMKL2015 - 0.6 waardelijsten.xlsx
@@ -1399,15 +1399,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1416,7 +1416,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="657225" y="352424"/>
+          <a:off x="647700" y="619124"/>
           <a:ext cx="4229100" cy="3209925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>